<commit_message>
test: modified test for #labels in spec
Modified named_cells.xslx to add in four named ranges: column_range, row_range, grid_range and non_adjacent_range.

Each tests named ranges in some way, with the most complex being the non_adjancet_range which can be a combination of single cells with grouped cells.
</commit_message>
<xml_diff>
--- a/test/files/named_cells.xlsx
+++ b/test/files/named_cells.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtishatter/Documents/Programming/roo/test/files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="308"/>
+    <workbookView xWindow="-34320" yWindow="3380" windowWidth="25140" windowHeight="15960" tabRatio="308"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,13 +20,25 @@
     <definedName name="anton">Sheet1!$C$5</definedName>
     <definedName name="berta">Sheet1!$B$4</definedName>
     <definedName name="caesar">Sheet1!$B$7</definedName>
+    <definedName name="column_range">Sheet1!$D$5:$D$9</definedName>
+    <definedName name="grid_range">Sheet1!$B$13:$D$14</definedName>
+    <definedName name="non_adjacent_range">Sheet1!$B$11:$D$11,Sheet1!$B$13:$D$14,Sheet1!$D$5:$D$9</definedName>
+    <definedName name="row_range">Sheet1!$B$11:$D$11</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Bertha</t>
   </si>
@@ -30,6 +47,48 @@
   </si>
   <si>
     <t>Cäsar</t>
+  </si>
+  <si>
+    <t>column_range_1</t>
+  </si>
+  <si>
+    <t>column_range_2</t>
+  </si>
+  <si>
+    <t>column_range_3</t>
+  </si>
+  <si>
+    <t>column_range_4</t>
+  </si>
+  <si>
+    <t>column_range_5</t>
+  </si>
+  <si>
+    <t>grid_range_1_1</t>
+  </si>
+  <si>
+    <t>grid_range_1_2</t>
+  </si>
+  <si>
+    <t>grid_range_2_1</t>
+  </si>
+  <si>
+    <t>grid_range_2_2</t>
+  </si>
+  <si>
+    <t>grid_range_3_1</t>
+  </si>
+  <si>
+    <t>grid_range_3_2</t>
+  </si>
+  <si>
+    <t>row_range_1</t>
+  </si>
+  <si>
+    <t>row_range_2</t>
+  </si>
+  <si>
+    <t>row_range_3</t>
   </si>
 </sst>
 </file>
@@ -67,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -451,27 +510,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:C7"/>
+  <dimension ref="B4:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
       <c r="C5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -489,9 +602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -507,9 +620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>